<commit_message>
Added framing, motor access, mold holder
</commit_message>
<xml_diff>
--- a/BOM/BOM_june12.xlsx
+++ b/BOM/BOM_june12.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jordan_Robarts\Spinning_Jig_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jordan_Robarts\Spinning_Jig_Project\Cardiac-Organ\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>BOM #</t>
   </si>
@@ -41,21 +41,9 @@
     <t xml:space="preserve">Quantity </t>
   </si>
   <si>
-    <t>Routing Clamps</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#8874t45/=181d9uf</t>
-  </si>
-  <si>
-    <t>Securing the DC motor to frame</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
-    <t>1.5 inch</t>
-  </si>
-  <si>
     <t>T Slotted Handle</t>
   </si>
   <si>
@@ -65,18 +53,6 @@
     <t>Handles for external frame</t>
   </si>
   <si>
-    <t>Routing Clamp Chain</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#1213n1/=181el9h</t>
-  </si>
-  <si>
-    <t>0.5 inch</t>
-  </si>
-  <si>
-    <t>Securing DC Motor to frame</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
@@ -108,6 +84,84 @@
   </si>
   <si>
     <t>Spacer for rotary shafts</t>
+  </si>
+  <si>
+    <t>T Slotted Framing</t>
+  </si>
+  <si>
+    <t>6.5 inch</t>
+  </si>
+  <si>
+    <t>8.5 inch</t>
+  </si>
+  <si>
+    <t>9.5 inch</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#47065t801/=186kah1</t>
+  </si>
+  <si>
+    <t>Inner gantry</t>
+  </si>
+  <si>
+    <t>12.5 inch</t>
+  </si>
+  <si>
+    <t>Inner-most gantry</t>
+  </si>
+  <si>
+    <t>Threaded Rod</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#95412a445/=186jmbp</t>
+  </si>
+  <si>
+    <t>3 INCH</t>
+  </si>
+  <si>
+    <t>1 (PACK OF 10)</t>
+  </si>
+  <si>
+    <t>Securing mold to gantry</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#2454K23</t>
+  </si>
+  <si>
+    <t>4 Arm Threaded Knob</t>
+  </si>
+  <si>
+    <t>10-32</t>
+  </si>
+  <si>
+    <t>1 (PACK OF 50)</t>
+  </si>
+  <si>
+    <t>S.S. Hex Nut</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#91841a195/=186kkom</t>
+  </si>
+  <si>
+    <t>3/8 inch</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/1084</t>
+  </si>
+  <si>
+    <t>DC Motor L-Bracket</t>
+  </si>
+  <si>
+    <t>Securing DC motor</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/2258</t>
+  </si>
+  <si>
+    <t>Stepper Motor L-Bracket</t>
+  </si>
+  <si>
+    <t>Securing Stepper Motor</t>
   </si>
 </sst>
 </file>
@@ -117,7 +171,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,13 +194,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -158,17 +232,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,204 +530,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="5" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="25.140625" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>17</v>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F2" s="5"/>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" s="2">
-        <f>3.14*B2</f>
-        <v>3.14</v>
+        <f>6.4*B2</f>
+        <v>12.8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5"/>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H3" s="2">
-        <f>6.4*B3</f>
-        <v>12.8</v>
+        <v>4.29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.192</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H4" s="2">
-        <v>3.46</v>
+        <v>4.4400000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
       </c>
+      <c r="F5" s="5"/>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H5" s="2">
-        <v>4.29</v>
+        <f>0.57*7</f>
+        <v>3.9899999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6">
-        <v>0.192</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F6" s="5"/>
       <c r="G6" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="2">
-        <v>4.4400000000000004</v>
+        <f>0.57*9</f>
+        <v>5.13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="2">
+        <v>7.42</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="2">
+        <f>4*2.65</f>
+        <v>10.6</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="2">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="2">
+        <v>4.95</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" location="47065t164/=181dc2a"/>
-    <hyperlink ref="D2" r:id="rId2" location="8874t45/=181d9uf"/>
+    <hyperlink ref="D2" r:id="rId1" location="47065t164/=181dc2a"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added rails after finalizing design
</commit_message>
<xml_diff>
--- a/BOM/BOM_june12.xlsx
+++ b/BOM/BOM_june12.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
   <si>
     <t>BOM #</t>
   </si>
@@ -59,15 +59,9 @@
     <t>MXL Timing Belt</t>
   </si>
   <si>
-    <t>https://www.mcmaster.com/#7887k79/=181f1p1</t>
-  </si>
-  <si>
     <t>Length</t>
   </si>
   <si>
-    <t>8 inch</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
@@ -95,18 +89,9 @@
     <t>8.5 inch</t>
   </si>
   <si>
-    <t>9.5 inch</t>
-  </si>
-  <si>
     <t>https://www.mcmaster.com/#47065t801/=186kah1</t>
   </si>
   <si>
-    <t>Inner gantry</t>
-  </si>
-  <si>
-    <t>12.5 inch</t>
-  </si>
-  <si>
     <t>Inner-most gantry</t>
   </si>
   <si>
@@ -143,9 +128,6 @@
     <t>https://www.mcmaster.com/#91841a195/=186kkom</t>
   </si>
   <si>
-    <t>3/8 inch</t>
-  </si>
-  <si>
     <t>https://www.pololu.com/product/1084</t>
   </si>
   <si>
@@ -162,6 +144,114 @@
   </si>
   <si>
     <t>Securing Stepper Motor</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#47065t854/=188kx18</t>
+  </si>
+  <si>
+    <t>Mounting plate (3"x3")</t>
+  </si>
+  <si>
+    <t>Securing Stepper to Rig</t>
+  </si>
+  <si>
+    <t>Mounting plate (3" x 1.5")</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#47065t853/=188kxoe</t>
+  </si>
+  <si>
+    <t>DC motor circuit/MCU</t>
+  </si>
+  <si>
+    <t>Mounting plate (2" x 2")</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#47065t852/=188kyri</t>
+  </si>
+  <si>
+    <t>2x2</t>
+  </si>
+  <si>
+    <t>3x1.5</t>
+  </si>
+  <si>
+    <t>3x3</t>
+  </si>
+  <si>
+    <t>DC Motor mount</t>
+  </si>
+  <si>
+    <t>1.5 inch</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#47065t801/=186kah2</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#47065t801/=186kah3</t>
+  </si>
+  <si>
+    <t>Outer gantry</t>
+  </si>
+  <si>
+    <t>10 inch</t>
+  </si>
+  <si>
+    <t>8.25 inch</t>
+  </si>
+  <si>
+    <t>Frame</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#47065t801/=186kah4</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#47065t801/=186kah5</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#47065t801/=186kah6</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#47065t801/=186kah7</t>
+  </si>
+  <si>
+    <t>16 inch</t>
+  </si>
+  <si>
+    <t>7 inch</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#6484k117/=188lfci</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#7887k77/=188lfzt</t>
+  </si>
+  <si>
+    <t>7.2 inch</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#7887k81/=188lrs3</t>
+  </si>
+  <si>
+    <t>9.6 inch</t>
+  </si>
+  <si>
+    <t>Belt for stepper</t>
+  </si>
+  <si>
+    <t>14.5 inch</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#5537T51</t>
+  </si>
+  <si>
+    <t>Framing Brace</t>
+  </si>
+  <si>
+    <t>1 inch</t>
+  </si>
+  <si>
+    <t>Framing brace</t>
   </si>
 </sst>
 </file>
@@ -171,7 +261,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,8 +299,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +316,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -238,15 +340,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -530,18 +645,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="8" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="25.140625" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="2"/>
@@ -560,8 +675,8 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>12</v>
+      <c r="E1" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
@@ -586,8 +701,8 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
+      <c r="E2" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" t="s">
@@ -608,241 +723,526 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>13</v>
+      <c r="D3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H3" s="2">
         <v>4.29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5</v>
-      </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.192</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="5"/>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2">
-        <v>4.4400000000000004</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>6</v>
-      </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="H5" s="2">
-        <f>0.57*7</f>
-        <v>3.9899999999999998</v>
+        <v>4.37</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.192</v>
+      </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H6" s="2">
-        <f>0.57*9</f>
-        <v>5.13</v>
+        <v>4.4400000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="H7" s="2">
+        <f>0.57*7*2</f>
+        <v>7.9799999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="H8" s="2">
+        <f>0.57*9*B8</f>
+        <v>10.26</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="2">
+        <f>0.57*2*4</f>
+        <v>4.5599999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="2">
+        <f>10*0.57*2</f>
+        <v>11.399999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="2">
+        <f>12*0.57*2</f>
+        <v>13.68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="2">
+        <f>4*9*0.57</f>
+        <v>20.52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="2">
+        <f>2*7*0.57</f>
+        <v>7.9799999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="2">
+        <f>15*0.57*2</f>
+        <v>17.099999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="2">
+        <f>16*0.57*2</f>
+        <v>18.239999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f>20+4+4+8</f>
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="2">
+        <f>5.51*B16</f>
+        <v>198.35999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E17" s="9"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" s="2">
+        <v>7.42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="E19" s="9">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="2">
-        <v>7.42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="2">
+      <c r="G19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="2">
         <f>4*2.65</f>
         <v>10.6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
         <v>36</v>
       </c>
-      <c r="C11" t="s">
+      <c r="H21" s="2">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
         <v>37</v>
       </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="2">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="H22" s="2">
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23">
         <v>1</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C23" t="s">
         <v>41</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D23" t="s">
         <v>40</v>
       </c>
-      <c r="G12" t="s">
+      <c r="E23" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="2">
-        <v>7.95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="H23" s="2">
+        <v>12.56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
         <v>44</v>
       </c>
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="E24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="2">
-        <v>4.95</v>
+      <c r="H24" s="2">
+        <v>12.14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="2">
+        <v>11.32</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H32" s="2">
+        <f>SUM(H2:H25)</f>
+        <v>410.59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" location="47065t164/=181dc2a"/>
+    <hyperlink ref="D25" r:id="rId2" location="47065t852/=188kyri"/>
+    <hyperlink ref="D3" r:id="rId3" location="6484k117/=188lfci"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added batteries and additional brace source
</commit_message>
<xml_diff>
--- a/BOM/BOM_june12.xlsx
+++ b/BOM/BOM_june12.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="98">
   <si>
     <t>BOM #</t>
   </si>
@@ -252,6 +252,72 @@
   </si>
   <si>
     <t>Framing brace</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/panasonic-bsg/KR1800SCEL5X2/SY156-L052-ND/1985934</t>
+  </si>
+  <si>
+    <t>8.33 inch</t>
+  </si>
+  <si>
+    <t>Battery for stepper and DC motor</t>
+  </si>
+  <si>
+    <t>https://elmwoodelectronics.ca/products/lithium-ion-polymer-battery-3-7v-500mah</t>
+  </si>
+  <si>
+    <t>LiPoly Battery 3.V 500 mAh</t>
+  </si>
+  <si>
+    <t>NiCad Battery 12 Volt  1800 mAh</t>
+  </si>
+  <si>
+    <t>1.15 inch</t>
+  </si>
+  <si>
+    <t>Battery for MCUs</t>
+  </si>
+  <si>
+    <t>NiCad Battery Charger (180 mA)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/XCSOURCE-Battery-Discharger-Charging-RC194/dp/B01FXD4ITM/ref=sr_1_14?ie=UTF8&amp;qid=1498663037&amp;sr=8-14&amp;keywords=nicd+battery+charger</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Charging for NiCad Bat</t>
+  </si>
+  <si>
+    <t>JST Cable Set</t>
+  </si>
+  <si>
+    <t>https://elmwoodelectronics.ca/products/2-pin-jst-sm-plug-receptacle-cable-set</t>
+  </si>
+  <si>
+    <t>16 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For NiCd Battery </t>
+  </si>
+  <si>
+    <t>Framing Bracket</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/products</t>
+  </si>
+  <si>
+    <t>SKU Code</t>
+  </si>
+  <si>
+    <t>27 mm</t>
+  </si>
+  <si>
+    <t>M5 Nuts</t>
+  </si>
+  <si>
+    <t>https://makerparts.ca/collections/screws-hardware/products/tee-nuts-25-pack</t>
   </si>
 </sst>
 </file>
@@ -261,7 +327,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,8 +371,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1C1B1A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +403,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -334,13 +418,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -362,8 +447,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="6" fillId="4" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Accent4" xfId="4" builtinId="41"/>
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -645,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +751,7 @@
     <col min="8" max="8" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -687,10 +776,13 @@
       <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -713,9 +805,9 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -737,7 +829,10 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4">
         <v>1</v>
       </c>
@@ -758,7 +853,10 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5">
         <v>1</v>
       </c>
@@ -779,7 +877,7 @@
         <v>4.37</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -805,7 +903,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -829,8 +927,9 @@
         <f>0.57*7*2</f>
         <v>7.9799999999999995</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -855,7 +954,7 @@
         <v>10.26</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -880,7 +979,7 @@
         <v>4.5599999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -905,7 +1004,7 @@
         <v>11.399999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -930,7 +1029,7 @@
         <v>13.68</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -955,7 +1054,7 @@
         <v>20.52</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -980,7 +1079,7 @@
         <v>7.9799999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1005,7 +1104,7 @@
         <v>17.099999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1030,37 +1129,61 @@
         <v>18.239999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="2">
+        <f>36*2.93</f>
+        <v>105.48</v>
+      </c>
+      <c r="I16" s="13">
+        <v>957416</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <f>20+4+4+8</f>
         <v>36</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>73</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" t="s">
+      <c r="F17" s="5"/>
+      <c r="G17" t="s">
         <v>75</v>
       </c>
-      <c r="H16" s="2">
-        <f>5.51*B16</f>
+      <c r="H17" s="12">
+        <f>5.51*B17</f>
         <v>198.35999999999999</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E17" s="9"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
       <c r="B18" t="s">
         <v>26</v>
       </c>
@@ -1083,7 +1206,10 @@
         <v>7.42</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
       <c r="B19">
         <v>4</v>
       </c>
@@ -1107,7 +1233,10 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -1130,7 +1259,10 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
       <c r="B21">
         <v>1</v>
       </c>
@@ -1150,7 +1282,10 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
       <c r="B22">
         <v>1</v>
       </c>
@@ -1170,7 +1305,10 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
       <c r="B23">
         <v>1</v>
       </c>
@@ -1190,7 +1328,10 @@
         <v>12.56</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
       <c r="B24">
         <v>1</v>
       </c>
@@ -1210,7 +1351,10 @@
         <v>12.14</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
       <c r="B25">
         <v>1</v>
       </c>
@@ -1230,10 +1374,123 @@
         <v>11.32</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="2">
+        <f>72.43*2</f>
+        <v>144.86000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" t="s">
+        <v>83</v>
+      </c>
+      <c r="H27" s="2">
+        <f>11.99*2</f>
+        <v>23.98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" s="2">
+        <v>34.99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="2">
+        <f>3.49*2</f>
+        <v>6.98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="2">
+        <f>SUM(H2:H26)</f>
+        <v>660.93000000000006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" t="s">
+        <v>97</v>
+      </c>
       <c r="H32" s="2">
-        <f>SUM(H2:H25)</f>
-        <v>410.59</v>
+        <f>7.99*2</f>
+        <v>15.98</v>
       </c>
     </row>
   </sheetData>
@@ -1241,8 +1498,9 @@
     <hyperlink ref="D2" r:id="rId1" location="47065t164/=181dc2a"/>
     <hyperlink ref="D25" r:id="rId2" location="47065t852/=188kyri"/>
     <hyperlink ref="D3" r:id="rId3" location="6484k117/=188lfci"/>
+    <hyperlink ref="D28" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalized all CAD files
</commit_message>
<xml_diff>
--- a/BOM/BOM_june12.xlsx
+++ b/BOM/BOM_june12.xlsx
@@ -209,9 +209,6 @@
     <t>14.5 inch</t>
   </si>
   <si>
-    <t>https://www.mcmaster.com/#5537T51</t>
-  </si>
-  <si>
     <t>Framing Brace</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>3/16</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#47065t216/=18jckzp</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +759,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3">
         <v>12.2</v>
@@ -783,14 +783,14 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4">
         <v>20</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H4" s="2">
         <v>5.77</v>
@@ -1056,17 +1056,17 @@
         <v>40</v>
       </c>
       <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="D15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H15" s="2">
         <f>5.51*B15</f>
@@ -1084,13 +1084,13 @@
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G16" t="s">
         <v>26</v>
@@ -1110,13 +1110,13 @@
         <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17" s="9">
         <v>0</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s">
         <v>26</v>
@@ -1137,13 +1137,13 @@
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" s="9">
         <v>0</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
         <v>26</v>
@@ -1276,16 +1276,16 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="G24" t="s">
         <v>66</v>
-      </c>
-      <c r="G24" t="s">
-        <v>67</v>
       </c>
       <c r="H24" s="2">
         <f>72.43*2</f>
@@ -1300,16 +1300,16 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" t="s">
         <v>71</v>
-      </c>
-      <c r="G25" t="s">
-        <v>72</v>
       </c>
       <c r="H25" s="2">
         <f>11.99*2</f>
@@ -1324,16 +1324,16 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="8" t="s">
+      <c r="G26" t="s">
         <v>74</v>
-      </c>
-      <c r="G26" t="s">
-        <v>75</v>
       </c>
       <c r="H26" s="2">
         <v>43.99</v>
@@ -1347,16 +1347,16 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="G27" t="s">
         <v>78</v>
-      </c>
-      <c r="G27" t="s">
-        <v>79</v>
       </c>
       <c r="H27" s="2">
         <f>3.49*2</f>
@@ -1371,16 +1371,16 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" t="s">
         <v>85</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="G28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H28" s="2">
         <f>3.49*2</f>
@@ -1395,16 +1395,16 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D29" t="s">
-        <v>88</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="G29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H29" s="2">
         <f>2*4.59</f>
@@ -1419,16 +1419,16 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E30" s="8">
         <v>0.2</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H30" s="2">
         <f>3.12*8</f>
@@ -1448,8 +1448,9 @@
     <hyperlink ref="D17" r:id="rId3" location="5993k13/=18dol11"/>
     <hyperlink ref="D27" r:id="rId4"/>
     <hyperlink ref="D24" r:id="rId5"/>
+    <hyperlink ref="D15" r:id="rId6" location="47065t216/=18jckzp"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>